<commit_message>
Se actualizaron los graficos de ambas clases.
</commit_message>
<xml_diff>
--- a/TP2/GráficosBinomioDeNewton.xlsx
+++ b/TP2/GráficosBinomioDeNewton.xlsx
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +42,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -60,10 +86,40 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -72,7 +128,7 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -85,38 +141,28 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -125,8 +171,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -135,9 +183,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -146,36 +198,48 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="60% - Énfasis1" xfId="2" builtinId="32"/>
+    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -205,9 +269,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -223,46 +286,121 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$12</c:f>
+              <c:f>Hoja1!$B$3:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>45321</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2365</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2365</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2759</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3153</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2758</c:v>
+                  <c:v>1417</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2365</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4729</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2365</c:v>
+                  <c:v>2267</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2364</c:v>
+                  <c:v>2552</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2835</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3118</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3402</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3685</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3686</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -278,46 +416,121 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$12</c:f>
+              <c:f>Hoja1!$D$3:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>10640</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7094</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2365</c:v>
+                  <c:v>1417</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2364</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2365</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2364</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2365</c:v>
+                  <c:v>1418</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2758</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2365</c:v>
+                  <c:v>1985</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1971</c:v>
+                  <c:v>1701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1417</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1701</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -327,21 +540,23 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="84436864"/>
-        <c:axId val="84438400"/>
-      </c:barChart>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="108066304"/>
+        <c:axId val="108067840"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="84436864"/>
+        <c:axId val="108066304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84438400"/>
+        <c:crossAx val="108067840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -349,7 +564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84438400"/>
+        <c:axId val="108067840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84436864"/>
+        <c:crossAx val="108066304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -386,16 +601,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -704,249 +919,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45321</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>10640</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="A3" s="5">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1701</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1701</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>2365</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>7094</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="A4" s="5">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1701</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1701</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2365</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2365</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="A5" s="5">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1701</v>
+      </c>
+      <c r="C5" s="5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1417</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>2759</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2364</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="A6" s="5">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1700</v>
+      </c>
+      <c r="C6" s="5">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1701</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>3153</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2365</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="A7" s="5">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1700</v>
+      </c>
+      <c r="C7" s="5">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1701</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2758</v>
-      </c>
-      <c r="C8" s="3">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2364</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="A8" s="5">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1417</v>
+      </c>
+      <c r="C8" s="5">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1701</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4">
-        <v>2365</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2365</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="A9" s="8">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1701</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1418</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>4729</v>
-      </c>
-      <c r="C10" s="3">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2758</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="A10" s="8">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1701</v>
+      </c>
+      <c r="C10" s="8">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1700</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2365</v>
-      </c>
-      <c r="C11" s="3">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2365</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>10</v>
+      <c r="A11" s="8">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2267</v>
+      </c>
+      <c r="C11" s="8">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>40</v>
       </c>
       <c r="B12" s="6">
-        <v>2364</v>
-      </c>
-      <c r="C12" s="5">
-        <v>10</v>
+        <v>2552</v>
+      </c>
+      <c r="C12" s="8">
+        <v>40</v>
       </c>
       <c r="D12" s="6">
-        <v>1971</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>50</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2835</v>
+      </c>
+      <c r="C13" s="8">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>60</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3118</v>
+      </c>
+      <c r="C14" s="8">
+        <v>60</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>70</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3402</v>
+      </c>
+      <c r="C15" s="8">
+        <v>70</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>80</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3685</v>
+      </c>
+      <c r="C16" s="8">
+        <v>80</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>90</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3686</v>
+      </c>
+      <c r="C17" s="8">
+        <v>90</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>200</v>
+      </c>
+      <c r="B18" s="10">
+        <v>8504</v>
+      </c>
+      <c r="C18" s="9">
+        <v>200</v>
+      </c>
+      <c r="D18" s="12">
+        <v>10773</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>